<commit_message>
Signed-off-by: James Schacht <pascal888@yahoo.com>
</commit_message>
<xml_diff>
--- a/Profit/Budget 2016 - itsprinting.org.xlsx
+++ b/Profit/Budget 2016 - itsprinting.org.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Total Expenses</t>
   </si>
@@ -152,6 +152,625 @@
   </si>
   <si>
     <t>Fundraising costs</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1% surcharge on all crowdsourced funding for projects that utilize the vPMO function of the Business Adopters community</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Average project: $20,000 funding</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Gross average $200 per project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note1: Higher volume is the goal – we can scale the site to handle the volume at greater efficiency due to scale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>iii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note2: Initial costs will be high due to development needed. Infrastructure costs can be incremented through a back-end agreement with organizations such as Parse.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Click-through advertising</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>The “Connections” section of 3DP Diner has a social networking feature that allows logical grouping of business contexts such as Consumer-to-Consumer (C2C), Business-to-Business (B2B), and Business-to-Consumer (B2C).  Within those constructs is a marketplace concept.  Permitting tasteful advertising in these contexts provides a revenue stream based on purchases made or services exchanged.  [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>quantify</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Targeted inbound advertising</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Utilize advanced analytics to target blogs and other quality content provided to direct custom advertising.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>This is a big field and can be very lucrative if done right</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>This can also challenge our principles and must be managed carefully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Donations from individuals</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Trades and Professions community members are offered a free skills profile they can store on our cloud.  We will have an API that makes this profile available to potential employers and other collaborators.  They have the option to donate when signing up for the community.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">They also have education options presented as part of the skills tool – this is free too, but offers another opportunity for an optional </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>donation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>The option to donate is also given to Business Adopters and Enthusiasts at community sign up time.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Donations from organizations and institutions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>One of our founding principles is to capture and share data and information gathered from our website, applications, and organizational programs.  We will seek grants and other monies that help us to do this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>We will accept donations from for-profit corporations if we can assure full transparency and absolutely no preferential treatment.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Developing business processes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>The blog DIMx3 captures the development of a process to utilize 3D printing to visualize large data sets.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Licensing – if we are successful in the development we could license it to businesses</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>There is a shortage of standards for 3D printing.  We could provide services in this sector and bill the consumer of the services.</t>
+    </r>
+  </si>
+  <si>
+    <t>vPMO Surcharge</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>10 projects average/month.  This will start out slower and pickup towards the end of the year.</t>
+  </si>
+  <si>
+    <t>Inbound Advertising</t>
+  </si>
+  <si>
+    <t>Fundraising Campaigns</t>
+  </si>
+  <si>
+    <t>Two major campaigns per year.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>(Checksum)</t>
+  </si>
+  <si>
+    <t>Marketplace Advertising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grants and Donations - Corporate </t>
+  </si>
+  <si>
+    <t>Grants and Donations - Individual</t>
+  </si>
+  <si>
+    <t>Inviduals</t>
+  </si>
+  <si>
+    <t>IT Services</t>
+  </si>
+  <si>
+    <t>Legal, CPA, Other administrative</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Revenue Category</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>In-kind</t>
+  </si>
+  <si>
+    <t>fees</t>
+  </si>
+  <si>
+    <t>license and association</t>
+  </si>
+  <si>
+    <t>assoc of 3D printing</t>
   </si>
 </sst>
 </file>
@@ -165,7 +784,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -286,6 +905,35 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -467,7 +1115,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -539,14 +1187,46 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -883,8 +1563,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -899,42 +1579,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
       <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="19"/>
       <c r="G4" s="15"/>
     </row>
@@ -971,7 +1651,7 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="50" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="22"/>
@@ -1009,7 +1689,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="23">
-        <v>11000</v>
+        <v>46000</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -1045,7 +1725,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="23">
-        <v>11000</v>
+        <v>46000</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
@@ -1057,7 +1737,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="23">
-        <v>99000</v>
+        <v>64000</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1069,7 +1749,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="23">
-        <v>99000</v>
+        <v>64000</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -1100,7 +1780,7 @@
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="49" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="24">
@@ -1162,7 +1842,7 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="51" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="26"/>
@@ -1353,7 +2033,7 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="49" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="24">
@@ -1459,15 +2139,548 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="66" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="57" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="57" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="64" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="66">
+        <v>1250</v>
+      </c>
+      <c r="C2" s="66">
+        <f>B2*12</f>
+        <v>15000</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="66">
+        <v>1200</v>
+      </c>
+      <c r="C3" s="66">
+        <f t="shared" ref="C3:C34" si="0">B3*12</f>
+        <v>14400</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="61"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="66">
+        <v>2884</v>
+      </c>
+      <c r="C4" s="66">
+        <f>B4*12</f>
+        <v>34608</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="61"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="66">
+        <v>5333</v>
+      </c>
+      <c r="C5" s="66">
+        <f t="shared" si="0"/>
+        <v>63996</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="66">
+        <v>3830</v>
+      </c>
+      <c r="C6" s="66">
+        <f t="shared" si="0"/>
+        <v>45960</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="61"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="66">
+        <v>3830</v>
+      </c>
+      <c r="C7" s="66">
+        <f t="shared" si="0"/>
+        <v>45960</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="61"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="66">
+        <v>420</v>
+      </c>
+      <c r="C8" s="66">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="66">
+        <v>420</v>
+      </c>
+      <c r="C9" s="66">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="61"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="61"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="61"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="61"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="61"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="61"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="61"/>
+    </row>
+    <row r="17" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="61"/>
+    </row>
+    <row r="18" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="61"/>
+    </row>
+    <row r="19" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="61"/>
+    </row>
+    <row r="20" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="61"/>
+    </row>
+    <row r="21" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="61"/>
+    </row>
+    <row r="22" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="61"/>
+    </row>
+    <row r="23" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="61"/>
+    </row>
+    <row r="24" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="61"/>
+    </row>
+    <row r="26" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="61"/>
+    </row>
+    <row r="27" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="61"/>
+    </row>
+    <row r="28" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="61"/>
+    </row>
+    <row r="29" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="61"/>
+    </row>
+    <row r="30" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="61"/>
+    </row>
+    <row r="31" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="61"/>
+    </row>
+    <row r="32" spans="3:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="61"/>
+    </row>
+    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="61"/>
+    </row>
+    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="61"/>
+    </row>
+    <row r="35" spans="1:5" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="67">
+        <f>SUM(B2:B34)</f>
+        <v>19167</v>
+      </c>
+      <c r="C35" s="67">
+        <f>SUM(C2:C34)</f>
+        <v>230004</v>
+      </c>
+      <c r="D35" s="53">
+        <f>B35*12</f>
+        <v>230004</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
+      <c r="E36" s="57"/>
+    </row>
+    <row r="37" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="E37" s="57"/>
+    </row>
+    <row r="38" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="E38" s="57"/>
+    </row>
+    <row r="39" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="E39" s="57"/>
+    </row>
+    <row r="40" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="E40" s="57"/>
+    </row>
+    <row r="41" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="E41" s="57"/>
+    </row>
+    <row r="42" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="E42" s="57"/>
+    </row>
+    <row r="43" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="E43" s="57"/>
+    </row>
+    <row r="44" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="E44" s="57"/>
+    </row>
+    <row r="45" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="68"/>
+      <c r="C45" s="68"/>
+      <c r="E45" s="57"/>
+    </row>
+    <row r="46" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="68"/>
+      <c r="C46" s="68"/>
+      <c r="E46" s="57"/>
+    </row>
+    <row r="47" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="68"/>
+      <c r="C47" s="68"/>
+      <c r="E47" s="57"/>
+    </row>
+    <row r="48" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="68"/>
+      <c r="C48" s="68"/>
+      <c r="E48" s="57"/>
+    </row>
+    <row r="49" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="68"/>
+      <c r="C49" s="68"/>
+      <c r="E49" s="57"/>
+    </row>
+    <row r="50" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="68"/>
+      <c r="C50" s="68"/>
+      <c r="E50" s="57"/>
+    </row>
+    <row r="51" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="68"/>
+      <c r="C51" s="68"/>
+      <c r="E51" s="57"/>
+    </row>
+    <row r="52" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="68"/>
+      <c r="C52" s="68"/>
+      <c r="E52" s="57"/>
+    </row>
+    <row r="53" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="68"/>
+      <c r="C53" s="68"/>
+      <c r="E53" s="57"/>
+    </row>
+    <row r="54" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="68"/>
+      <c r="C54" s="68"/>
+      <c r="E54" s="57"/>
+    </row>
+    <row r="55" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="68"/>
+      <c r="C55" s="68"/>
+      <c r="E55" s="57"/>
+    </row>
+    <row r="56" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="68"/>
+      <c r="C56" s="68"/>
+      <c r="E56" s="57"/>
+    </row>
+    <row r="57" spans="1:5" s="61" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="E57" s="57"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1476,12 +2689,26 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>